<commit_message>
Added 256 core runs to benchmark
</commit_message>
<xml_diff>
--- a/taito_benchmark.xlsx
+++ b/taito_benchmark.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
   <si>
     <t>Mitsuba Taito benchmark</t>
   </si>
@@ -234,6 +234,36 @@
   </si>
   <si>
     <t>The light image seemingly doesn't affect CPU utilization!</t>
+  </si>
+  <si>
+    <t>29 G</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>8k</t>
+  </si>
+  <si>
+    <t>eta 2,9m</t>
+  </si>
+  <si>
+    <t>limit (15)</t>
+  </si>
+  <si>
+    <t>4,02 G</t>
+  </si>
+  <si>
+    <t>20,26 G</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>12,9 M</t>
+  </si>
+  <si>
+    <t>16,67 G</t>
   </si>
 </sst>
 </file>
@@ -565,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,6 +605,7 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -773,39 +804,39 @@
         <v>12</v>
       </c>
       <c r="F7">
-        <f>F6*F5</f>
+        <f t="shared" ref="F7:N7" si="0">F6*F5</f>
         <v>1</v>
       </c>
       <c r="G7">
-        <f>G6*G5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H7">
-        <f>H6*H5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I7">
-        <f>I6*I5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J7">
-        <f>J6*J5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K7">
-        <f>K6*K5</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="L7">
-        <f>L6*L5</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="M7">
-        <f>M6*M5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="N7">
-        <f>N6*N5</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="O7">
@@ -822,11 +853,11 @@
         <v>16</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:T7" si="0">S6*S5</f>
+        <f t="shared" ref="S7:T7" si="1">S6*S5</f>
         <v>16</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
     </row>
@@ -1225,15 +1256,15 @@
         <v>16</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:J24" si="1">G23*G22</f>
+        <f t="shared" ref="G24:I24" si="2">G23*G22</f>
         <v>64</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
     </row>
@@ -1271,7 +1302,7 @@
         <v>154.26599999999999</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I26" si="2">60*I25</f>
+        <f t="shared" ref="I26" si="3">60*I25</f>
         <v>546</v>
       </c>
     </row>
@@ -1491,7 +1522,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1527,8 +1558,11 @@
       <c r="J50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1553,8 +1587,11 @@
       <c r="J51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1579,8 +1616,11 @@
       <c r="J52">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1592,23 +1632,27 @@
         <v>16</v>
       </c>
       <c r="G53">
-        <f t="shared" ref="G53:K53" si="3">G52*G51</f>
+        <f t="shared" ref="G53:I53" si="4">G52*G51</f>
         <v>16</v>
       </c>
       <c r="H53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="I53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="J53">
         <f>J52*J51</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <f>K52*K51</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>13</v>
       </c>
@@ -1627,8 +1671,11 @@
       <c r="J54">
         <v>28.084199999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="3">
+        <v>10.957700000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
         <v>14</v>
       </c>
@@ -1641,11 +1688,11 @@
         <v>580.70399999999995</v>
       </c>
       <c r="H55">
-        <f t="shared" ref="H55:K55" si="4">60*H54</f>
+        <f t="shared" ref="H55:I55" si="5">60*H54</f>
         <v>314.42400000000004</v>
       </c>
       <c r="I55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>314.41199999999998</v>
       </c>
       <c r="J55">
@@ -1653,7 +1700,7 @@
         <v>1685.0519999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>17</v>
       </c>
@@ -1672,8 +1719,11 @@
       <c r="J56">
         <v>84.14</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="1">
+        <v>63.99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>18</v>
       </c>
@@ -1692,8 +1742,11 @@
       <c r="J57">
         <v>1950</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>19</v>
       </c>
@@ -1712,8 +1765,11 @@
       <c r="J58" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>7</v>
       </c>
@@ -1732,13 +1788,19 @@
       <c r="J59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I60" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1749,7 +1811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1771,8 +1833,14 @@
       <c r="J63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <v>20</v>
+      </c>
+      <c r="L63">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1794,8 +1862,14 @@
       <c r="J64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <v>20</v>
+      </c>
+      <c r="L64">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -1817,8 +1891,14 @@
       <c r="J65">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <v>16</v>
+      </c>
+      <c r="L65">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1830,19 +1910,27 @@
         <v>16</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66" si="5">G65*G64</f>
+        <f t="shared" ref="G66" si="6">G65*G64</f>
         <v>16</v>
       </c>
       <c r="H66">
-        <f t="shared" ref="H66" si="6">H65*H64</f>
+        <f t="shared" ref="H66" si="7">H65*H64</f>
         <v>32</v>
       </c>
       <c r="J66">
         <f>J65*J64</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <f>K65*K64</f>
+        <v>320</v>
+      </c>
+      <c r="L66">
+        <f>L65*L64</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
         <v>13</v>
       </c>
@@ -1858,8 +1946,14 @@
       <c r="J67">
         <v>32.767200000000003</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L67" s="3">
+        <v>13.1717</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
         <v>14</v>
       </c>
@@ -1872,15 +1966,19 @@
         <v>663.678</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68" si="7">60*H67</f>
+        <f t="shared" ref="H68" si="8">60*H67</f>
         <v>361.67399999999998</v>
       </c>
       <c r="J68">
         <f>60*J67</f>
         <v>1966.0320000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <f>60*L67</f>
+        <v>790.30200000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>17</v>
       </c>
@@ -1890,14 +1988,20 @@
       <c r="G69">
         <v>95.75</v>
       </c>
-      <c r="H69" s="1">
+      <c r="H69" s="3">
         <v>88.79</v>
       </c>
-      <c r="J69" s="1">
+      <c r="J69" s="3">
         <v>85.15</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="1">
+        <v>55.47</v>
+      </c>
+      <c r="L69" s="1">
+        <v>63.83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>18</v>
       </c>
@@ -1913,8 +2017,14 @@
       <c r="J70">
         <v>2600</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" t="s">
+        <v>70</v>
+      </c>
+      <c r="L70" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>19</v>
       </c>
@@ -1924,14 +2034,20 @@
       <c r="G71" t="s">
         <v>16</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H71" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="J71" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" t="s">
+        <v>71</v>
+      </c>
+      <c r="L71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>7</v>
       </c>
@@ -1947,8 +2063,19 @@
       <c r="J72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" t="s">
+        <v>72</v>
+      </c>
+      <c r="L72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E74" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Added kitchen2 pt128 benchmark
</commit_message>
<xml_diff>
--- a/taito_benchmark.xlsx
+++ b/taito_benchmark.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
   <si>
     <t>Mitsuba Taito benchmark</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>16,67 G</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>12,2 M</t>
+  </si>
+  <si>
+    <t>Bad util for simple pt</t>
   </si>
 </sst>
 </file>
@@ -593,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U74"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,6 +2089,121 @@
         <v>69</v>
       </c>
     </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81">
+        <f>F80*F79</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82">
+        <v>9.6265000000000001</v>
+      </c>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83">
+        <f>60*F82</f>
+        <v>577.59</v>
+      </c>
+    </row>
+    <row r="84" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>17</v>
+      </c>
+      <c r="F84" s="1">
+        <v>75.48</v>
+      </c>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85">
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="86" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E89" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added ideal CPU eff. calculation
</commit_message>
<xml_diff>
--- a/taito_benchmark.xlsx
+++ b/taito_benchmark.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="93">
   <si>
     <t>Mitsuba Taito benchmark</t>
   </si>
@@ -273,6 +273,36 @@
   </si>
   <si>
     <t>Bad util for simple pt</t>
+  </si>
+  <si>
+    <t>Triton</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>10,28 M</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>1 idle</t>
+  </si>
+  <si>
+    <t>12,40 M</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Setup time (s)</t>
+  </si>
+  <si>
+    <t>Optimal eff</t>
+  </si>
+  <si>
+    <t>Opimal eff</t>
   </si>
 </sst>
 </file>
@@ -316,12 +346,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U89"/>
+  <dimension ref="A1:U95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +645,9 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -995,6 +1028,12 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
@@ -1045,177 +1084,220 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="F11">
-        <v>51.02</v>
+        <f>(100/(F4*F6) + 500*(F4-1)/(F4*F6) + 100*$B$10/(F4*F6) + 100*F9)/(1+5+$B$10+F9)</f>
+        <v>99.376684510111417</v>
       </c>
       <c r="G11">
-        <v>57.92</v>
+        <f>(100/(G4*G6) + 500*(G4-1)/(G4*G6) + 100*$B$10/(G4*G6) + 100*G9)/(1+5+$B$10+G9)</f>
+        <v>98.545976231558129</v>
       </c>
       <c r="H11">
-        <v>116.57</v>
+        <f t="shared" ref="H11:T11" si="2">(100/(H4*H6) + 500*(H4-1)/(H4*H6) + 100*$B$10/(H4*H6) + 100*H9)/(1+5+$B$10+H9)</f>
+        <v>99.273536383373525</v>
       </c>
       <c r="I11">
-        <v>289.17</v>
+        <f t="shared" si="2"/>
+        <v>98.807779348137103</v>
       </c>
       <c r="J11">
-        <v>71.7</v>
+        <f t="shared" si="2"/>
+        <v>97.17187187274294</v>
       </c>
       <c r="K11">
-        <v>693.55</v>
+        <f>(100/(K4*K6) + 500*(K4-1)/(K4*K6) + 100*$B$10/(K4*K6) + 100*K9)/(1+5+$B$10+K9)</f>
+        <v>83.821321321321321</v>
       </c>
       <c r="L11">
-        <v>1150</v>
+        <f t="shared" si="2"/>
+        <v>86.847696970938216</v>
       </c>
       <c r="M11">
-        <v>130.4</v>
+        <f t="shared" si="2"/>
+        <v>97.676929476003792</v>
       </c>
       <c r="N11">
-        <v>360.84</v>
+        <f t="shared" si="2"/>
+        <v>91.594943518020443</v>
       </c>
       <c r="O11">
-        <v>639.16999999999996</v>
+        <f t="shared" si="2"/>
+        <v>84.39816745436012</v>
       </c>
       <c r="P11">
-        <v>533.47</v>
+        <f t="shared" si="2"/>
+        <v>86.261424374719496</v>
       </c>
       <c r="Q11">
-        <v>539.30999999999995</v>
-      </c>
-      <c r="R11" s="3">
-        <v>2440</v>
+        <f t="shared" si="2"/>
+        <v>89.16902552390755</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>97.070600208908061</v>
       </c>
       <c r="S11">
-        <v>154.36000000000001</v>
+        <f t="shared" si="2"/>
+        <v>89.269046466979873</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>99.227950111891715</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>51.02</v>
+      </c>
+      <c r="G12">
+        <v>57.92</v>
+      </c>
+      <c r="H12">
+        <v>116.57</v>
+      </c>
+      <c r="I12">
+        <v>289.17</v>
+      </c>
+      <c r="J12">
+        <v>71.7</v>
+      </c>
+      <c r="K12">
+        <v>693.55</v>
+      </c>
+      <c r="L12">
+        <v>1150</v>
+      </c>
+      <c r="M12">
+        <v>130.4</v>
+      </c>
+      <c r="N12">
+        <v>360.84</v>
+      </c>
+      <c r="O12">
+        <v>639.16999999999996</v>
+      </c>
+      <c r="P12">
+        <v>533.47</v>
+      </c>
+      <c r="Q12">
+        <v>539.30999999999995</v>
+      </c>
+      <c r="R12" s="3">
+        <v>2440</v>
+      </c>
+      <c r="S12">
+        <v>154.36000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>30</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>26</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O14" t="s">
         <v>49</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P14" t="s">
         <v>50</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q14" t="s">
         <v>51</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T14" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E15" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>4</v>
-      </c>
-      <c r="H21">
-        <v>4</v>
-      </c>
-      <c r="I21">
-        <v>8</v>
+        <v>68</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1232,246 +1314,290 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H23">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I23">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="G24">
+        <v>16</v>
+      </c>
+      <c r="H24">
+        <v>16</v>
+      </c>
+      <c r="I24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>66</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>12</v>
       </c>
-      <c r="F24">
-        <f>F23*F22</f>
-        <v>16</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ref="G24:I24" si="2">G23*G22</f>
+      <c r="F25">
+        <f>F24*F23</f>
+        <v>16</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:I25" si="3">G24*G23</f>
         <v>64</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="2"/>
+      <c r="H25">
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="2"/>
+      <c r="I25">
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>13</v>
       </c>
-      <c r="F25">
-        <f>F26/60</f>
+      <c r="F26">
+        <f>F27/60</f>
         <v>0.93446666666666667</v>
       </c>
-      <c r="G25">
-        <f>G26/60</f>
+      <c r="G26">
+        <f>G27/60</f>
         <v>0.26241666666666663</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>2.5710999999999999</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <v>9.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26">
-        <v>56.067999999999998</v>
-      </c>
-      <c r="G26">
-        <v>15.744999999999999</v>
-      </c>
-      <c r="H26">
-        <f>60*H25</f>
-        <v>154.26599999999999</v>
-      </c>
-      <c r="I26">
-        <f t="shared" ref="I26" si="3">60*I25</f>
-        <v>546</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F27">
-        <v>88.1</v>
+        <v>56.067999999999998</v>
       </c>
       <c r="G27">
-        <v>63.52</v>
+        <v>15.744999999999999</v>
       </c>
       <c r="H27">
-        <v>88.18</v>
+        <f>60*H26</f>
+        <v>154.26599999999999</v>
       </c>
       <c r="I27">
-        <v>81.3</v>
-      </c>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
+        <f t="shared" ref="I27" si="4">60*I26</f>
+        <v>546</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28">
-        <v>27.15</v>
-      </c>
-      <c r="G28" t="s">
-        <v>37</v>
+        <v>88.1</v>
+      </c>
+      <c r="G28">
+        <v>63.52</v>
       </c>
       <c r="H28">
-        <v>114.12</v>
+        <v>88.18</v>
       </c>
       <c r="I28">
-        <v>242.6</v>
-      </c>
+        <v>81.3</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
       <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" t="s">
-        <v>39</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F29">
+        <f>(100/(F22*F24) + 500*(F22-1)/(F22*F24) + 100*$B$26/(F22*F24) + 100*F27)/(1+5+$B$26+F27)</f>
+        <v>89.099067672987886</v>
+      </c>
+      <c r="G29">
+        <f>(100/(G22*G24) + 500*(G22-1)/(G22*G24) + 100*$B$26/(G22*G24) + 100*G27)/(1+5+$B$26+G27)</f>
+        <v>70.391844361398114</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:I29" si="5">(100/(H22*H24) + 500*(H22-1)/(H22*H24) + 100*$B$26/(H22*H24) + 100*H27)/(1+5+$B$26+H27)</f>
+        <v>95.824057767911398</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>98.786448915009046</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <v>27.15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30">
+        <v>114.12</v>
+      </c>
+      <c r="I30">
+        <v>242.6</v>
+      </c>
+      <c r="T30" s="3"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" t="s">
+        <v>39</v>
+      </c>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>26</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H32" t="s">
         <v>35</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I32" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>66</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E38" t="s">
         <v>11</v>
       </c>
-      <c r="F36">
-        <v>16</v>
-      </c>
-      <c r="G36">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
+      <c r="F38">
+        <v>16</v>
+      </c>
+      <c r="G38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="4">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
         <v>12</v>
       </c>
-      <c r="F37">
-        <f>F36*F35</f>
-        <v>16</v>
-      </c>
-      <c r="G37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38">
-        <v>17.593399999999999</v>
-      </c>
-      <c r="G38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
-        <v>14</v>
+      <c r="F39">
+        <f>F38*F37</f>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
         <v>16</v>
@@ -1479,10 +1605,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F40">
-        <v>95.95</v>
+        <v>17.593399999999999</v>
       </c>
       <c r="G40" t="s">
         <v>16</v>
@@ -1490,10 +1616,11 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F41">
-        <v>921.73</v>
+        <f>60*F40</f>
+        <v>1055.604</v>
       </c>
       <c r="G41" t="s">
         <v>16</v>
@@ -1501,10 +1628,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F42">
+        <v>95.95</v>
       </c>
       <c r="G42" t="s">
         <v>16</v>
@@ -1512,696 +1639,956 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43">
+        <f>(100/(F36*F38) + 500*(F36-1)/(F36*F38) + 100*$B$39/(F36*F38) + 100*F41)/(1+5+$B$39+F41)</f>
+        <v>98.057032082286256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44">
+        <v>921.73</v>
+      </c>
+      <c r="G44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
         <v>7</v>
       </c>
-      <c r="F43">
+      <c r="F46">
         <v>512</v>
       </c>
-      <c r="G43">
+      <c r="G46">
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G44" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E46" s="1" t="s">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="2" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E53" t="s">
         <v>9</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50">
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
         <v>2</v>
       </c>
-      <c r="I50">
+      <c r="I53">
         <v>2</v>
       </c>
-      <c r="J50">
-        <v>4</v>
-      </c>
-      <c r="K50">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="J53">
+        <v>4</v>
+      </c>
+      <c r="K53">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E54" t="s">
         <v>10</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
         <v>2</v>
       </c>
-      <c r="I51">
+      <c r="I54">
         <v>2</v>
       </c>
-      <c r="J51">
-        <v>4</v>
-      </c>
-      <c r="K51">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E55" t="s">
         <v>11</v>
       </c>
-      <c r="F52">
-        <v>16</v>
-      </c>
-      <c r="G52">
-        <v>16</v>
-      </c>
-      <c r="H52">
-        <v>16</v>
-      </c>
-      <c r="I52">
-        <v>16</v>
-      </c>
-      <c r="J52">
-        <v>16</v>
-      </c>
-      <c r="K52">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="F55">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>16</v>
+      </c>
+      <c r="H55">
+        <v>16</v>
+      </c>
+      <c r="I55">
+        <v>16</v>
+      </c>
+      <c r="J55">
+        <v>16</v>
+      </c>
+      <c r="K55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>66</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E56" t="s">
         <v>12</v>
       </c>
-      <c r="F53">
-        <f>F52*F51</f>
-        <v>16</v>
-      </c>
-      <c r="G53">
-        <f t="shared" ref="G53:I53" si="4">G52*G51</f>
-        <v>16</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="4"/>
+      <c r="F56">
+        <f>F55*F54</f>
+        <v>16</v>
+      </c>
+      <c r="G56">
+        <f t="shared" ref="G56:I56" si="6">G55*G54</f>
+        <v>16</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="4"/>
+      <c r="I56">
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="J53">
-        <f>J52*J51</f>
+      <c r="J56">
+        <f>J55*J54</f>
         <v>64</v>
       </c>
-      <c r="K53">
-        <f>K52*K51</f>
+      <c r="K56">
+        <f>K55*K54</f>
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="4">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
         <v>13</v>
       </c>
-      <c r="F54">
+      <c r="F57">
         <v>1.2444</v>
       </c>
-      <c r="G54">
+      <c r="G57">
         <v>9.6783999999999999</v>
       </c>
-      <c r="H54">
+      <c r="H57">
         <v>5.2404000000000002</v>
       </c>
-      <c r="I54">
+      <c r="I57">
         <v>5.2401999999999997</v>
       </c>
-      <c r="J54">
+      <c r="J57">
         <v>28.084199999999999</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K57" s="3">
         <v>10.957700000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
         <v>14</v>
       </c>
-      <c r="F55">
-        <f>60*F54</f>
+      <c r="F58">
+        <f>60*F57</f>
         <v>74.664000000000001</v>
       </c>
-      <c r="G55">
-        <f>60*G54</f>
+      <c r="G58">
+        <f>60*G57</f>
         <v>580.70399999999995</v>
       </c>
-      <c r="H55">
-        <f t="shared" ref="H55:I55" si="5">60*H54</f>
+      <c r="H58">
+        <f t="shared" ref="H58:I58" si="7">60*H57</f>
         <v>314.42400000000004</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="5"/>
+      <c r="I58">
+        <f t="shared" si="7"/>
         <v>314.41199999999998</v>
       </c>
-      <c r="J55">
-        <f>60*J54</f>
+      <c r="J58">
+        <f>60*J57</f>
         <v>1685.0519999999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
+      <c r="K58">
+        <f>60*K57</f>
+        <v>657.4620000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
         <v>17</v>
       </c>
-      <c r="F56">
+      <c r="F59">
         <v>79.37</v>
       </c>
-      <c r="G56">
+      <c r="G59">
         <v>95.84</v>
       </c>
-      <c r="H56">
+      <c r="H59">
         <v>82.7</v>
       </c>
-      <c r="I56">
+      <c r="I59">
         <v>87.21</v>
       </c>
-      <c r="J56">
+      <c r="J59">
         <v>84.14</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K59" s="1">
         <v>63.99</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E57" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60">
+        <f>(100/(F53*F55) + 500*(F53-1)/(F53*F55) + 100*$B$57/(F53*F55) + 100*F58)/(1+5+$B$57+F58)</f>
+        <v>78.339919721923366</v>
+      </c>
+      <c r="G60">
+        <f t="shared" ref="G60:K60" si="8">(100/(G53*G55) + 500*(G53-1)/(G53*G55) + 100*$B$57/(G53*G55) + 100*G58)/(1+5+$B$57+G58)</f>
+        <v>96.526072499933633</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="8"/>
+        <v>93.664988229139425</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="8"/>
+        <v>93.664762255805385</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="8"/>
+        <v>98.740518742252718</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="8"/>
+        <v>96.815035277911051</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
         <v>18</v>
       </c>
-      <c r="F57">
+      <c r="F61">
         <v>318.91000000000003</v>
       </c>
-      <c r="G57">
+      <c r="G61">
         <v>311.44</v>
       </c>
-      <c r="H57">
+      <c r="H61">
         <v>827.8</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I61" t="s">
         <v>63</v>
       </c>
-      <c r="J57">
+      <c r="J61">
         <v>1950</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E58" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
         <v>19</v>
       </c>
-      <c r="F58" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" t="s">
-        <v>16</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="F62" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" t="s">
         <v>58</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I62" t="s">
         <v>62</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J62" t="s">
         <v>60</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K62" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E59" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
         <v>7</v>
       </c>
-      <c r="F59">
+      <c r="F63">
         <v>64</v>
       </c>
-      <c r="G59">
+      <c r="G63">
         <v>500</v>
       </c>
-      <c r="H59">
+      <c r="H63">
         <v>500</v>
       </c>
-      <c r="I59">
+      <c r="I63">
         <v>500</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J63" t="s">
         <v>59</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I60" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
         <v>61</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K64" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>2</v>
-      </c>
-      <c r="J63">
-        <v>4</v>
-      </c>
-      <c r="K63">
-        <v>20</v>
-      </c>
-      <c r="L63">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
-      <c r="H64">
-        <v>2</v>
-      </c>
-      <c r="J64">
-        <v>4</v>
-      </c>
-      <c r="K64">
-        <v>20</v>
-      </c>
-      <c r="L64">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E65" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65">
-        <v>16</v>
-      </c>
-      <c r="G65">
-        <v>16</v>
-      </c>
-      <c r="H65">
-        <v>16</v>
-      </c>
-      <c r="J65">
-        <v>16</v>
-      </c>
-      <c r="K65">
-        <v>16</v>
-      </c>
-      <c r="L65">
-        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+      <c r="K67">
+        <v>20</v>
+      </c>
+      <c r="L67">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="J68">
+        <v>4</v>
+      </c>
+      <c r="K68">
+        <v>20</v>
+      </c>
+      <c r="L68">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>55</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69">
+        <v>16</v>
+      </c>
+      <c r="G69">
+        <v>16</v>
+      </c>
+      <c r="H69">
+        <v>16</v>
+      </c>
+      <c r="J69">
+        <v>16</v>
+      </c>
+      <c r="K69">
+        <v>16</v>
+      </c>
+      <c r="L69">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>65</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E70" t="s">
         <v>12</v>
       </c>
-      <c r="F66">
-        <f>F65*F64</f>
-        <v>16</v>
-      </c>
-      <c r="G66">
-        <f t="shared" ref="G66" si="6">G65*G64</f>
-        <v>16</v>
-      </c>
-      <c r="H66">
-        <f t="shared" ref="H66" si="7">H65*H64</f>
+      <c r="F70">
+        <f>F69*F68</f>
+        <v>16</v>
+      </c>
+      <c r="G70">
+        <f t="shared" ref="G70" si="9">G69*G68</f>
+        <v>16</v>
+      </c>
+      <c r="H70">
+        <f t="shared" ref="H70" si="10">H69*H68</f>
         <v>32</v>
       </c>
-      <c r="J66">
-        <f>J65*J64</f>
+      <c r="J70">
+        <f>J69*J68</f>
         <v>64</v>
       </c>
-      <c r="K66">
-        <f>K65*K64</f>
+      <c r="K70">
+        <f>K69*K68</f>
         <v>320</v>
       </c>
-      <c r="L66">
-        <f>L65*L64</f>
+      <c r="L70">
+        <f>L69*L68</f>
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
+    <row r="71" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="4">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
         <v>13</v>
       </c>
-      <c r="F67">
+      <c r="F71">
         <v>1.4516</v>
       </c>
-      <c r="G67">
+      <c r="G71">
         <v>11.061299999999999</v>
       </c>
-      <c r="H67">
+      <c r="H71">
         <v>6.0278999999999998</v>
       </c>
-      <c r="J67">
+      <c r="J71">
         <v>32.767200000000003</v>
       </c>
-      <c r="K67" s="3" t="s">
+      <c r="K71" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L71" s="3">
         <v>13.1717</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68">
-        <f>60*F67</f>
-        <v>87.096000000000004</v>
-      </c>
-      <c r="G68">
-        <f>60*G67</f>
-        <v>663.678</v>
-      </c>
-      <c r="H68">
-        <f t="shared" ref="H68" si="8">60*H67</f>
-        <v>361.67399999999998</v>
-      </c>
-      <c r="J68">
-        <f>60*J67</f>
-        <v>1966.0320000000002</v>
-      </c>
-      <c r="L68">
-        <f>60*L67</f>
-        <v>790.30200000000002</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
-        <v>17</v>
-      </c>
-      <c r="F69">
-        <v>80.2</v>
-      </c>
-      <c r="G69">
-        <v>95.75</v>
-      </c>
-      <c r="H69" s="3">
-        <v>88.79</v>
-      </c>
-      <c r="J69" s="3">
-        <v>85.15</v>
-      </c>
-      <c r="K69" s="1">
-        <v>55.47</v>
-      </c>
-      <c r="L69" s="1">
-        <v>63.83</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70">
-        <v>440.02</v>
-      </c>
-      <c r="G70">
-        <v>437.05</v>
-      </c>
-      <c r="H70">
-        <v>1080</v>
-      </c>
-      <c r="J70">
-        <v>2600</v>
-      </c>
-      <c r="K70" t="s">
-        <v>70</v>
-      </c>
-      <c r="L70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" t="s">
-        <v>16</v>
-      </c>
-      <c r="G71" t="s">
-        <v>16</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K71" t="s">
-        <v>71</v>
-      </c>
-      <c r="L71" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72">
+        <f>60*F71</f>
+        <v>87.096000000000004</v>
+      </c>
+      <c r="G72">
+        <f>60*G71</f>
+        <v>663.678</v>
+      </c>
+      <c r="H72">
+        <f t="shared" ref="H72" si="11">60*H71</f>
+        <v>361.67399999999998</v>
+      </c>
+      <c r="J72">
+        <f>60*J71</f>
+        <v>1966.0320000000002</v>
+      </c>
+      <c r="K72" s="5">
+        <f>60*15</f>
+        <v>900</v>
+      </c>
+      <c r="L72">
+        <f>60*L71</f>
+        <v>790.30200000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73">
+        <v>80.2</v>
+      </c>
+      <c r="G73">
+        <v>95.75</v>
+      </c>
+      <c r="H73" s="3">
+        <v>88.79</v>
+      </c>
+      <c r="J73" s="3">
+        <v>85.15</v>
+      </c>
+      <c r="K73" s="1">
+        <v>55.47</v>
+      </c>
+      <c r="L73" s="1">
+        <v>63.83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>92</v>
+      </c>
+      <c r="F74">
+        <f>(100/(F67*F69) + 500*(F67-1)/(F67*F69) + 100*$B$71/(F67*F69) + 100*F72)/(1+5+$B$71+F72)</f>
+        <v>80.808187284593387</v>
+      </c>
+      <c r="G74">
+        <f t="shared" ref="G74:L74" si="12">(100/(G67*G69) + 500*(G67-1)/(G67*G69) + 100*$B$71/(G67*G69) + 100*G72)/(1+5+$B$71+G72)</f>
+        <v>96.946452999804578</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="12"/>
+        <v>94.445153958829621</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="12"/>
+        <v>98.918528474390754</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="12"/>
+        <v>97.651843817787423</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="12"/>
+        <v>97.335889238238977</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75">
+        <v>440.02</v>
+      </c>
+      <c r="G75">
+        <v>437.05</v>
+      </c>
+      <c r="H75">
+        <v>1080</v>
+      </c>
+      <c r="J75">
+        <v>2600</v>
+      </c>
+      <c r="K75" t="s">
+        <v>70</v>
+      </c>
+      <c r="L75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K76" t="s">
+        <v>71</v>
+      </c>
+      <c r="L76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
         <v>7</v>
       </c>
-      <c r="F72">
+      <c r="F77">
         <v>64</v>
       </c>
-      <c r="G72">
+      <c r="G77">
         <v>500</v>
       </c>
-      <c r="H72">
+      <c r="H77">
         <v>500</v>
       </c>
-      <c r="J72" t="s">
+      <c r="J77" t="s">
         <v>59</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K77" t="s">
         <v>72</v>
       </c>
-      <c r="L72" t="s">
+      <c r="L77" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K73" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K78" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E74" s="1" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E79" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>1</v>
-      </c>
-      <c r="B78" s="2" t="s">
+      <c r="M82" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E83" t="s">
         <v>9</v>
       </c>
-      <c r="F78">
+      <c r="F83">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="G83">
+        <v>8</v>
+      </c>
+      <c r="M83" t="s">
+        <v>9</v>
+      </c>
+      <c r="N83">
+        <v>4</v>
+      </c>
+      <c r="O83">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E84" t="s">
         <v>10</v>
       </c>
-      <c r="F79">
+      <c r="F84">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="G84">
+        <v>8</v>
+      </c>
+      <c r="M84" t="s">
+        <v>10</v>
+      </c>
+      <c r="N84">
+        <v>4</v>
+      </c>
+      <c r="O84">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>66</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E85" t="s">
         <v>11</v>
       </c>
-      <c r="F80">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="81" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E81" t="s">
+      <c r="F85">
+        <v>16</v>
+      </c>
+      <c r="G85">
+        <v>16</v>
+      </c>
+      <c r="M85" t="s">
+        <v>11</v>
+      </c>
+      <c r="N85">
         <v>12</v>
       </c>
-      <c r="F81">
-        <f>F80*F79</f>
+      <c r="O85">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" s="4">
+        <v>16</v>
+      </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86">
+        <f>F85*F84</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="82" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E82" t="s">
+      <c r="G86">
+        <f>G85*G84</f>
+        <v>128</v>
+      </c>
+      <c r="M86" t="s">
+        <v>12</v>
+      </c>
+      <c r="N86">
+        <f>N85*N84</f>
+        <v>48</v>
+      </c>
+      <c r="O86">
+        <f>O85*O84</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
         <v>13</v>
       </c>
-      <c r="F82">
+      <c r="F87">
         <v>9.6265000000000001</v>
       </c>
-      <c r="K82" s="3"/>
-    </row>
-    <row r="83" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E83" t="s">
+      <c r="M87" t="s">
+        <v>13</v>
+      </c>
+      <c r="N87">
+        <v>4.8578000000000001</v>
+      </c>
+      <c r="O87" s="3">
+        <v>4.3205999999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
         <v>14</v>
       </c>
-      <c r="F83">
-        <f>60*F82</f>
+      <c r="F88">
+        <f>60*F87</f>
         <v>577.59</v>
       </c>
-    </row>
-    <row r="84" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E84" t="s">
+      <c r="M88" t="s">
+        <v>14</v>
+      </c>
+      <c r="N88">
+        <f>60*N87</f>
+        <v>291.46800000000002</v>
+      </c>
+      <c r="O88">
+        <f>60*O87</f>
+        <v>259.23599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
         <v>17</v>
       </c>
-      <c r="F84" s="1">
+      <c r="F89" s="1">
         <v>75.48</v>
       </c>
-      <c r="K84" s="1"/>
-    </row>
-    <row r="85" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E85" t="s">
+      <c r="M89" t="s">
+        <v>17</v>
+      </c>
+      <c r="N89" s="3">
+        <v>83.57</v>
+      </c>
+      <c r="O89" s="1">
+        <v>74.53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>92</v>
+      </c>
+      <c r="F90">
+        <f>(100/(F83*F85) + 500*(F83-1)/(F83*F85) + 100*$B$86/(F83*F85) + 100*F88)/(1+5+$B$86+F88)</f>
+        <v>96.398580696809475</v>
+      </c>
+      <c r="M90" t="s">
+        <v>91</v>
+      </c>
+      <c r="N90">
+        <f>(100/(N83*N85) + 500*(N83-1)/(N83*N85) + 100*$B$86/(N83*N85) + 100*N88)/(1+5+$B$86+N88)</f>
+        <v>93.194414315549494</v>
+      </c>
+      <c r="O90">
+        <f>(100/(O83*O85) + 500*(O83-1)/(O83*O85) + 100*$B$86/(O83*O85) + 100*O88)/(1+5+$B$86+O88)</f>
+        <v>92.361101234076244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
         <v>18</v>
       </c>
-      <c r="F85">
+      <c r="F91">
         <v>5350</v>
       </c>
-    </row>
-    <row r="86" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E86" t="s">
+      <c r="M91" t="s">
+        <v>18</v>
+      </c>
+      <c r="N91">
+        <v>2330</v>
+      </c>
+      <c r="O91">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
         <v>19</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F92" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="87" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E87" t="s">
+      <c r="M92" t="s">
+        <v>19</v>
+      </c>
+      <c r="N92" t="s">
+        <v>85</v>
+      </c>
+      <c r="O92" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
         <v>7</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F93" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="89" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E89" s="1" t="s">
+      <c r="G93" t="s">
+        <v>80</v>
+      </c>
+      <c r="M93" t="s">
+        <v>7</v>
+      </c>
+      <c r="N93" t="s">
+        <v>84</v>
+      </c>
+      <c r="O93" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F94">
+        <v>43.73</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E95" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="G95" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Idle + master swap tests
</commit_message>
<xml_diff>
--- a/taito_benchmark.xlsx
+++ b/taito_benchmark.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="105">
   <si>
     <t>Mitsuba Taito benchmark</t>
   </si>
@@ -303,6 +303,55 @@
   </si>
   <si>
     <t>Opimal eff</t>
+  </si>
+  <si>
+    <t>3 idle</t>
+  </si>
+  <si>
+    <t>12,59 M</t>
+  </si>
+  <si>
+    <t>12,3 M</t>
+  </si>
+  <si>
+    <t>Faster??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Box, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 idle</t>
+    </r>
+  </si>
+  <si>
+    <t>Does affect time taken to render though!!</t>
+  </si>
+  <si>
+    <t>13,0 M</t>
+  </si>
+  <si>
+    <t>16,73 G</t>
+  </si>
+  <si>
+    <t>82,2 BU</t>
+  </si>
+  <si>
+    <t>Faster but lower util...?</t>
+  </si>
+  <si>
+    <t>Master swapped</t>
+  </si>
+  <si>
+    <t>12,265 M</t>
   </si>
 </sst>
 </file>
@@ -633,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U95"/>
+  <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T77" sqref="T77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,12 +1733,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E49" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1700,7 +1749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1728,8 +1777,11 @@
       <c r="K53">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1757,8 +1809,11 @@
       <c r="K54">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1786,8 +1841,11 @@
       <c r="K55">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -1818,8 +1876,12 @@
         <f>K55*K54</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <f>L55*L54</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>90</v>
       </c>
@@ -1847,8 +1909,14 @@
       <c r="K57" s="3">
         <v>10.957700000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="1">
+        <v>9.3109000000000002</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>14</v>
       </c>
@@ -1876,8 +1944,12 @@
         <f>60*K57</f>
         <v>657.4620000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <f>60*L57</f>
+        <v>558.654</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>17</v>
       </c>
@@ -1899,8 +1971,11 @@
       <c r="K59" s="1">
         <v>63.99</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="1">
+        <v>60.61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>91</v>
       </c>
@@ -1909,7 +1984,7 @@
         <v>78.339919721923366</v>
       </c>
       <c r="G60">
-        <f t="shared" ref="G60:K60" si="8">(100/(G53*G55) + 500*(G53-1)/(G53*G55) + 100*$B$57/(G53*G55) + 100*G58)/(1+5+$B$57+G58)</f>
+        <f t="shared" ref="G60:L60" si="8">(100/(G53*G55) + 500*(G53-1)/(G53*G55) + 100*$B$57/(G53*G55) + 100*G58)/(1+5+$B$57+G58)</f>
         <v>96.526072499933633</v>
       </c>
       <c r="H60">
@@ -1925,11 +2000,15 @@
         <v>98.740518742252718</v>
       </c>
       <c r="K60">
-        <f t="shared" si="8"/>
+        <f>(100/(K53*K55) + 500*(K53-1)/(K53*K55) + 100*$B$57/(K53*K55) + 100*K58)/(1+5+$B$57+K58)</f>
         <v>96.815035277911051</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <f>(100/(L53*L55) + 500*(L53-1)/(L53*L55) + 100*$B$57/(L53*L55) + 100*L58)/(1+5+$B$57+L58)</f>
+        <v>96.273060204528008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>18</v>
       </c>
@@ -1951,8 +2030,11 @@
       <c r="K61" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>19</v>
       </c>
@@ -1974,8 +2056,11 @@
       <c r="K62" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>7</v>
       </c>
@@ -1997,64 +2082,46 @@
       <c r="K63" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I64" t="s">
         <v>61</v>
       </c>
       <c r="K64" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>15</v>
+      <c r="L64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L65" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67">
-        <v>1</v>
-      </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="H67">
-        <v>2</v>
-      </c>
-      <c r="J67">
-        <v>4</v>
-      </c>
-      <c r="K67">
-        <v>20</v>
-      </c>
-      <c r="L67">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2077,28 +2144,28 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F69">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G69">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H69">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J69">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K69">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L69">
         <v>16</v>
@@ -2106,274 +2173,282 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70">
+        <v>16</v>
+      </c>
+      <c r="G70">
+        <v>16</v>
+      </c>
+      <c r="H70">
+        <v>16</v>
+      </c>
+      <c r="J70">
+        <v>16</v>
+      </c>
+      <c r="K70">
+        <v>16</v>
+      </c>
+      <c r="L70">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>65</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>12</v>
       </c>
-      <c r="F70">
-        <f>F69*F68</f>
-        <v>16</v>
-      </c>
-      <c r="G70">
-        <f t="shared" ref="G70" si="9">G69*G68</f>
-        <v>16</v>
-      </c>
-      <c r="H70">
-        <f t="shared" ref="H70" si="10">H69*H68</f>
+      <c r="F71">
+        <f>F70*F69</f>
+        <v>16</v>
+      </c>
+      <c r="G71">
+        <f t="shared" ref="G71" si="9">G70*G69</f>
+        <v>16</v>
+      </c>
+      <c r="H71">
+        <f t="shared" ref="H71" si="10">H70*H69</f>
         <v>32</v>
       </c>
-      <c r="J70">
-        <f>J69*J68</f>
+      <c r="J71">
+        <f>J70*J69</f>
         <v>64</v>
       </c>
-      <c r="K70">
-        <f>K69*K68</f>
+      <c r="K71">
+        <f>K70*K69</f>
         <v>320</v>
       </c>
-      <c r="L70">
-        <f>L69*L68</f>
+      <c r="L71">
+        <f>L70*L69</f>
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="72" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="4">
-        <v>16</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="B72" s="4">
+        <v>16</v>
+      </c>
+      <c r="E72" t="s">
         <v>13</v>
       </c>
-      <c r="F71">
+      <c r="F72">
         <v>1.4516</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>11.061299999999999</v>
       </c>
-      <c r="H71">
+      <c r="H72">
         <v>6.0278999999999998</v>
       </c>
-      <c r="J71">
+      <c r="J72">
         <v>32.767200000000003</v>
       </c>
-      <c r="K71" s="3" t="s">
+      <c r="K72" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L71" s="3">
+      <c r="L72" s="3">
         <v>13.1717</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
         <v>14</v>
       </c>
-      <c r="F72">
-        <f>60*F71</f>
+      <c r="F73">
+        <f>60*F72</f>
         <v>87.096000000000004</v>
       </c>
-      <c r="G72">
-        <f>60*G71</f>
+      <c r="G73">
+        <f>60*G72</f>
         <v>663.678</v>
       </c>
-      <c r="H72">
-        <f t="shared" ref="H72" si="11">60*H71</f>
+      <c r="H73">
+        <f t="shared" ref="H73" si="11">60*H72</f>
         <v>361.67399999999998</v>
       </c>
-      <c r="J72">
-        <f>60*J71</f>
+      <c r="J73">
+        <f>60*J72</f>
         <v>1966.0320000000002</v>
       </c>
-      <c r="K72" s="5">
+      <c r="K73" s="5">
         <f>60*15</f>
         <v>900</v>
       </c>
-      <c r="L72">
-        <f>60*L71</f>
+      <c r="L73">
+        <f>60*L72</f>
         <v>790.30200000000002</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
-        <v>17</v>
-      </c>
-      <c r="F73">
-        <v>80.2</v>
-      </c>
-      <c r="G73">
-        <v>95.75</v>
-      </c>
-      <c r="H73" s="3">
-        <v>88.79</v>
-      </c>
-      <c r="J73" s="3">
-        <v>85.15</v>
-      </c>
-      <c r="K73" s="1">
-        <v>55.47</v>
-      </c>
-      <c r="L73" s="1">
-        <v>63.83</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74">
+        <v>80.2</v>
+      </c>
+      <c r="G74">
+        <v>95.75</v>
+      </c>
+      <c r="H74" s="3">
+        <v>88.79</v>
+      </c>
+      <c r="J74" s="3">
+        <v>85.15</v>
+      </c>
+      <c r="K74" s="1">
+        <v>55.47</v>
+      </c>
+      <c r="L74" s="1">
+        <v>63.83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
         <v>92</v>
       </c>
-      <c r="F74">
-        <f>(100/(F67*F69) + 500*(F67-1)/(F67*F69) + 100*$B$71/(F67*F69) + 100*F72)/(1+5+$B$71+F72)</f>
+      <c r="F75">
+        <f>(100/(F68*F70) + 500*(F68-1)/(F68*F70) + 100*$B$72/(F68*F70) + 100*F73)/(1+5+$B$72+F73)</f>
         <v>80.808187284593387</v>
       </c>
-      <c r="G74">
-        <f t="shared" ref="G74:L74" si="12">(100/(G67*G69) + 500*(G67-1)/(G67*G69) + 100*$B$71/(G67*G69) + 100*G72)/(1+5+$B$71+G72)</f>
+      <c r="G75">
+        <f t="shared" ref="G75:L75" si="12">(100/(G68*G70) + 500*(G68-1)/(G68*G70) + 100*$B$72/(G68*G70) + 100*G73)/(1+5+$B$72+G73)</f>
         <v>96.946452999804578</v>
       </c>
-      <c r="H74">
+      <c r="H75">
         <f t="shared" si="12"/>
         <v>94.445153958829621</v>
       </c>
-      <c r="J74">
+      <c r="J75">
         <f t="shared" si="12"/>
         <v>98.918528474390754</v>
       </c>
-      <c r="K74">
+      <c r="K75">
         <f t="shared" si="12"/>
         <v>97.651843817787423</v>
       </c>
-      <c r="L74">
+      <c r="L75">
         <f t="shared" si="12"/>
         <v>97.335889238238977</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75">
-        <v>440.02</v>
-      </c>
-      <c r="G75">
-        <v>437.05</v>
-      </c>
-      <c r="H75">
-        <v>1080</v>
-      </c>
-      <c r="J75">
-        <v>2600</v>
-      </c>
-      <c r="K75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L75" t="s">
-        <v>76</v>
-      </c>
-    </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" t="s">
-        <v>16</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
+      </c>
+      <c r="F76">
+        <v>440.02</v>
+      </c>
+      <c r="G76">
+        <v>437.05</v>
+      </c>
+      <c r="H76">
+        <v>1080</v>
+      </c>
+      <c r="J76">
+        <v>2600</v>
       </c>
       <c r="K76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L76" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K77" t="s">
+        <v>71</v>
+      </c>
+      <c r="L77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
         <v>7</v>
       </c>
-      <c r="F77">
+      <c r="F78">
         <v>64</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <v>500</v>
       </c>
-      <c r="H77">
+      <c r="H78">
         <v>500</v>
       </c>
-      <c r="J77" t="s">
+      <c r="J78" t="s">
         <v>59</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K78" t="s">
         <v>72</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L78" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K78" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K79" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E79" s="1" t="s">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E81" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M82" s="1" t="s">
+      <c r="M83" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>1</v>
-      </c>
-      <c r="B83" s="2" t="s">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>9</v>
-      </c>
-      <c r="F83">
-        <v>8</v>
-      </c>
-      <c r="G83">
-        <v>8</v>
-      </c>
-      <c r="M83" t="s">
-        <v>9</v>
-      </c>
-      <c r="N83">
-        <v>4</v>
-      </c>
-      <c r="O83">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E84" t="s">
-        <v>10</v>
       </c>
       <c r="F84">
         <v>8</v>
@@ -2381,8 +2456,11 @@
       <c r="G84">
         <v>8</v>
       </c>
+      <c r="H84">
+        <v>8</v>
+      </c>
       <c r="M84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N84">
         <v>4</v>
@@ -2390,205 +2468,343 @@
       <c r="O84">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P84">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85">
+        <v>8</v>
+      </c>
+      <c r="G85">
+        <v>8</v>
+      </c>
+      <c r="H85">
+        <v>8</v>
+      </c>
+      <c r="M85" t="s">
+        <v>10</v>
+      </c>
+      <c r="N85">
+        <v>4</v>
+      </c>
+      <c r="O85">
+        <v>10</v>
+      </c>
+      <c r="P85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>66</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E86" t="s">
         <v>11</v>
       </c>
-      <c r="F85">
-        <v>16</v>
-      </c>
-      <c r="G85">
-        <v>16</v>
-      </c>
-      <c r="M85" t="s">
+      <c r="F86">
+        <v>16</v>
+      </c>
+      <c r="G86">
+        <v>16</v>
+      </c>
+      <c r="H86">
+        <v>16</v>
+      </c>
+      <c r="M86" t="s">
         <v>11</v>
       </c>
-      <c r="N85">
+      <c r="N86">
         <v>12</v>
       </c>
-      <c r="O85">
+      <c r="O86">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="P86">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>90</v>
       </c>
-      <c r="B86" s="4">
-        <v>16</v>
-      </c>
-      <c r="E86" t="s">
+      <c r="B87" s="4">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
         <v>12</v>
       </c>
-      <c r="F86">
-        <f>F85*F84</f>
+      <c r="F87">
+        <f>F86*F85</f>
         <v>128</v>
       </c>
-      <c r="G86">
-        <f>G85*G84</f>
+      <c r="G87">
+        <f>G86*G85</f>
         <v>128</v>
       </c>
-      <c r="M86" t="s">
+      <c r="H87">
+        <f>H86*H85</f>
+        <v>128</v>
+      </c>
+      <c r="M87" t="s">
         <v>12</v>
       </c>
-      <c r="N86">
-        <f>N85*N84</f>
+      <c r="N87">
+        <f>N86*N85</f>
         <v>48</v>
       </c>
-      <c r="O86">
-        <f>O85*O84</f>
+      <c r="O87">
+        <f>O86*O85</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E87" t="s">
+      <c r="P87">
+        <f>P86*P85</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
         <v>13</v>
       </c>
-      <c r="F87">
+      <c r="F88">
         <v>9.6265000000000001</v>
       </c>
-      <c r="M87" t="s">
+      <c r="G88" s="1">
+        <v>8.9794</v>
+      </c>
+      <c r="H88">
+        <v>8.7073999999999998</v>
+      </c>
+      <c r="M88" t="s">
         <v>13</v>
       </c>
-      <c r="N87">
+      <c r="N88">
         <v>4.8578000000000001</v>
       </c>
-      <c r="O87" s="3">
+      <c r="O88" s="3">
         <v>4.3205999999999998</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E88" t="s">
+      <c r="P88">
+        <v>4.3733000000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
         <v>14</v>
       </c>
-      <c r="F88">
-        <f>60*F87</f>
+      <c r="F89">
+        <f>60*F88</f>
         <v>577.59</v>
       </c>
-      <c r="M88" t="s">
+      <c r="G89">
+        <f>60*G88</f>
+        <v>538.76400000000001</v>
+      </c>
+      <c r="H89">
+        <f>60*H88</f>
+        <v>522.44399999999996</v>
+      </c>
+      <c r="M89" t="s">
         <v>14</v>
       </c>
-      <c r="N88">
-        <f>60*N87</f>
+      <c r="N89">
+        <f>60*N88</f>
         <v>291.46800000000002</v>
       </c>
-      <c r="O88">
-        <f>60*O87</f>
+      <c r="O89">
+        <f>60*O88</f>
         <v>259.23599999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E89" t="s">
+      <c r="P89">
+        <f>60*P88</f>
+        <v>262.39800000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
         <v>17</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F90" s="1">
         <v>75.48</v>
       </c>
-      <c r="M89" t="s">
+      <c r="G90" s="1">
+        <v>73.37</v>
+      </c>
+      <c r="H90">
+        <v>75.66</v>
+      </c>
+      <c r="M90" t="s">
         <v>17</v>
       </c>
-      <c r="N89" s="3">
+      <c r="N90" s="3">
         <v>83.57</v>
       </c>
-      <c r="O89" s="1">
+      <c r="O90" s="1">
         <v>74.53</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E90" t="s">
+      <c r="P90">
+        <v>75.33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
         <v>92</v>
       </c>
-      <c r="F90">
-        <f>(100/(F83*F85) + 500*(F83-1)/(F83*F85) + 100*$B$86/(F83*F85) + 100*F88)/(1+5+$B$86+F88)</f>
+      <c r="F91">
+        <f>(100/(F84*F86) + 500*(F84-1)/(F84*F86) + 100*$B$87/(F84*F86) + 100*F89)/(1+5+$B$87+F89)</f>
         <v>96.398580696809475</v>
       </c>
-      <c r="M90" t="s">
+      <c r="G91">
+        <f>(100/(G84*G86) + 500*(G84-1)/(G84*G86) + 100*$B$87/(G84*G86) + 100*G89)/(1+5+$B$87+G89)</f>
+        <v>96.149226769193461</v>
+      </c>
+      <c r="H91">
+        <f>(100/(G84*G86) + 500*(G84-1)/(G84*G86) + 100*$B$87/(G84*G86) + 100*G89)/(1+5+$B$87+G89)</f>
+        <v>96.149226769193461</v>
+      </c>
+      <c r="M91" t="s">
         <v>91</v>
       </c>
-      <c r="N90">
-        <f>(100/(N83*N85) + 500*(N83-1)/(N83*N85) + 100*$B$86/(N83*N85) + 100*N88)/(1+5+$B$86+N88)</f>
+      <c r="N91">
+        <f>(100/(N84*N86) + 500*(N84-1)/(N84*N86) + 100*$B$87/(N84*N86) + 100*N89)/(1+5+$B$87+N89)</f>
         <v>93.194414315549494</v>
       </c>
-      <c r="O90">
-        <f>(100/(O83*O85) + 500*(O83-1)/(O83*O85) + 100*$B$86/(O83*O85) + 100*O88)/(1+5+$B$86+O88)</f>
+      <c r="O91">
+        <f>(100/(O84*O86) + 500*(O84-1)/(O84*O86) + 100*$B$87/(O84*O86) + 100*O89)/(1+5+$B$87+O89)</f>
         <v>92.361101234076244</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E91" t="s">
+      <c r="P91">
+        <f>(100/(P84*P86) + 500*(P84-1)/(P84*P86) + 100*$B$87/(P84*P86) + 100*P89)/(1+5+$B$87+P89)</f>
+        <v>92.446032203695765</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
         <v>18</v>
       </c>
-      <c r="F91">
+      <c r="F92">
         <v>5350</v>
       </c>
-      <c r="M91" t="s">
+      <c r="G92">
+        <v>5430</v>
+      </c>
+      <c r="H92">
+        <v>5310</v>
+      </c>
+      <c r="M92" t="s">
         <v>18</v>
       </c>
-      <c r="N91">
+      <c r="N92">
         <v>2330</v>
       </c>
-      <c r="O91">
+      <c r="O92">
         <v>8600</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E92" t="s">
+      <c r="P92">
+        <v>8570</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
         <v>19</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F93" t="s">
         <v>81</v>
       </c>
-      <c r="M92" t="s">
+      <c r="G93" t="s">
+        <v>95</v>
+      </c>
+      <c r="H93" t="s">
+        <v>104</v>
+      </c>
+      <c r="M93" t="s">
         <v>19</v>
       </c>
-      <c r="N92" t="s">
+      <c r="N93" t="s">
         <v>85</v>
       </c>
-      <c r="O92" t="s">
+      <c r="O93" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E93" t="s">
+      <c r="P93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
         <v>7</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F94" t="s">
         <v>80</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" t="s">
         <v>80</v>
       </c>
-      <c r="M93" t="s">
+      <c r="H94" t="s">
+        <v>80</v>
+      </c>
+      <c r="M94" t="s">
         <v>7</v>
       </c>
-      <c r="N93" t="s">
+      <c r="N94" t="s">
         <v>84</v>
       </c>
-      <c r="O93" t="s">
+      <c r="O94" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E94" t="s">
+      <c r="P94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
         <v>86</v>
       </c>
-      <c r="F94">
+      <c r="F95">
         <v>43.73</v>
       </c>
-      <c r="O94" s="1" t="s">
+      <c r="G95">
+        <v>39.61</v>
+      </c>
+      <c r="H95">
+        <v>38.47</v>
+      </c>
+      <c r="O95" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E95" s="1" t="s">
+      <c r="P95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>87</v>
+      </c>
+      <c r="H96" t="s">
+        <v>87</v>
+      </c>
+      <c r="I96" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E97" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G95" t="s">
-        <v>87</v>
+      <c r="G97" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H97" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 16x16 block benchmark
</commit_message>
<xml_diff>
--- a/taito_benchmark.xlsx
+++ b/taito_benchmark.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="112">
   <si>
     <t>Mitsuba Taito benchmark</t>
   </si>
@@ -345,13 +345,34 @@
     <t>82,2 BU</t>
   </si>
   <si>
-    <t>Faster but lower util...?</t>
-  </si>
-  <si>
     <t>Master swapped</t>
   </si>
   <si>
     <t>12,265 M</t>
+  </si>
+  <si>
+    <t>Cputime/sample</t>
+  </si>
+  <si>
+    <t>Cpu_t/sample</t>
+  </si>
+  <si>
+    <t>cputime</t>
+  </si>
+  <si>
+    <t>16,69 G</t>
+  </si>
+  <si>
+    <t>16x16 blocks, 2 idle</t>
+  </si>
+  <si>
+    <t>60,3 BU</t>
+  </si>
+  <si>
+    <t>Conclusion: Make sure blocks &gt; cores * MTS_BACKLOG_FACTOR ( = 3)</t>
+  </si>
+  <si>
+    <t>14,259 M</t>
   </si>
 </sst>
 </file>
@@ -682,10 +703,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U97"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:U103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T77" sqref="T77"/>
+    <sheetView tabSelected="1" topLeftCell="E42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1599,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33">
+        <f>F25*F27/320</f>
+        <v>2.8033999999999999</v>
+      </c>
+      <c r="G33">
+        <f>G25*G27/320</f>
+        <v>3.149</v>
+      </c>
+      <c r="H33">
+        <f>H25*H27/3200</f>
+        <v>3.0853199999999998</v>
+      </c>
+      <c r="I33">
+        <f>I25*I27/20000</f>
+        <v>3.4944000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1586,7 +1631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1603,7 +1648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1620,7 +1665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -1634,7 +1679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -1652,7 +1697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>13</v>
       </c>
@@ -1663,7 +1708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>14</v>
       </c>
@@ -1675,7 +1720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>17</v>
       </c>
@@ -1686,7 +1731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>91</v>
       </c>
@@ -1695,7 +1740,7 @@
         <v>98.057032082286256</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>19</v>
       </c>
@@ -1717,7 +1762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>7</v>
       </c>
@@ -1728,7 +1773,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>48</v>
       </c>
@@ -1780,6 +1825,9 @@
       <c r="L53">
         <v>16</v>
       </c>
+      <c r="M53">
+        <v>16</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -1812,6 +1860,9 @@
       <c r="L54">
         <v>16</v>
       </c>
+      <c r="M54">
+        <v>16</v>
+      </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -1844,6 +1895,9 @@
       <c r="L55">
         <v>16</v>
       </c>
+      <c r="M55">
+        <v>16</v>
+      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1880,6 +1934,10 @@
         <f>L55*L54</f>
         <v>256</v>
       </c>
+      <c r="M56">
+        <f>M55*M54</f>
+        <v>256</v>
+      </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -1912,8 +1970,8 @@
       <c r="L57" s="1">
         <v>9.3109000000000002</v>
       </c>
-      <c r="M57" s="1" t="s">
-        <v>102</v>
+      <c r="M57" s="3">
+        <v>6.7648000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -1948,867 +2006,1031 @@
         <f>60*L57</f>
         <v>558.654</v>
       </c>
+      <c r="M58">
+        <f>60*M57</f>
+        <v>405.88800000000003</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="F59">
-        <v>79.37</v>
+        <f>F58*F56*F60/100</f>
+        <v>948.17306880000001</v>
       </c>
       <c r="G59">
-        <v>95.84</v>
+        <f t="shared" ref="G59:M59" si="8">G58*G56*G60/100</f>
+        <v>8904.7474175999996</v>
       </c>
       <c r="H59">
-        <v>82.7</v>
+        <f t="shared" si="8"/>
+        <v>8320.916736000001</v>
       </c>
       <c r="I59">
-        <v>87.21</v>
+        <f t="shared" si="8"/>
+        <v>8774.3585663999984</v>
       </c>
       <c r="J59">
-        <v>84.14</v>
-      </c>
-      <c r="K59" s="1">
-        <v>63.99</v>
-      </c>
-      <c r="L59" s="1">
-        <v>60.61</v>
+        <f t="shared" si="8"/>
+        <v>90739.3761792</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="8"/>
+        <v>107701.74305280001</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="8"/>
+        <v>86681.648486400009</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="8"/>
+        <v>85910.578790400003</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1">
+        <v>79.37</v>
+      </c>
+      <c r="G60" s="1">
+        <v>95.84</v>
+      </c>
+      <c r="H60">
+        <v>82.7</v>
+      </c>
+      <c r="I60">
+        <v>87.21</v>
+      </c>
+      <c r="J60">
+        <v>84.14</v>
+      </c>
+      <c r="K60" s="1">
+        <v>63.99</v>
+      </c>
+      <c r="L60" s="1">
+        <v>60.61</v>
+      </c>
+      <c r="M60">
+        <v>82.68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
         <v>91</v>
       </c>
-      <c r="F60">
+      <c r="F61">
         <f>(100/(F53*F55) + 500*(F53-1)/(F53*F55) + 100*$B$57/(F53*F55) + 100*F58)/(1+5+$B$57+F58)</f>
         <v>78.339919721923366</v>
       </c>
-      <c r="G60">
-        <f t="shared" ref="G60:L60" si="8">(100/(G53*G55) + 500*(G53-1)/(G53*G55) + 100*$B$57/(G53*G55) + 100*G58)/(1+5+$B$57+G58)</f>
+      <c r="G61">
+        <f t="shared" ref="G61:J61" si="9">(100/(G53*G55) + 500*(G53-1)/(G53*G55) + 100*$B$57/(G53*G55) + 100*G58)/(1+5+$B$57+G58)</f>
         <v>96.526072499933633</v>
       </c>
-      <c r="H60">
-        <f t="shared" si="8"/>
+      <c r="H61">
+        <f t="shared" si="9"/>
         <v>93.664988229139425</v>
       </c>
-      <c r="I60">
-        <f t="shared" si="8"/>
+      <c r="I61">
+        <f t="shared" si="9"/>
         <v>93.664762255805385</v>
       </c>
-      <c r="J60">
-        <f t="shared" si="8"/>
+      <c r="J61">
+        <f t="shared" si="9"/>
         <v>98.740518742252718</v>
       </c>
-      <c r="K60">
+      <c r="K61">
         <f>(100/(K53*K55) + 500*(K53-1)/(K53*K55) + 100*$B$57/(K53*K55) + 100*K58)/(1+5+$B$57+K58)</f>
         <v>96.815035277911051</v>
       </c>
-      <c r="L60">
+      <c r="L61">
         <f>(100/(L53*L55) + 500*(L53-1)/(L53*L55) + 100*$B$57/(L53*L55) + 100*L58)/(1+5+$B$57+L58)</f>
         <v>96.273060204528008</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E61" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61">
-        <v>318.91000000000003</v>
-      </c>
-      <c r="G61">
-        <v>311.44</v>
-      </c>
-      <c r="H61">
-        <v>827.8</v>
-      </c>
-      <c r="I61" t="s">
-        <v>63</v>
-      </c>
-      <c r="J61">
-        <v>1950</v>
-      </c>
-      <c r="K61" t="s">
-        <v>79</v>
-      </c>
-      <c r="L61" t="s">
-        <v>100</v>
+      <c r="M61">
+        <f>(100/(M53*M55) + 500*(M53-1)/(M53*M55) + 100*$B$57/(M53*M55) + 100*M58)/(1+5+$B$57+M58)</f>
+        <v>94.942455736080476</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H62" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="F62">
+        <v>318.91000000000003</v>
+      </c>
+      <c r="G62">
+        <v>311.44</v>
+      </c>
+      <c r="H62">
+        <v>827.8</v>
       </c>
       <c r="I62" t="s">
-        <v>62</v>
-      </c>
-      <c r="J62" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="J62">
+        <v>1950</v>
       </c>
       <c r="K62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L62" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="M62" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" t="s">
+        <v>58</v>
+      </c>
+      <c r="I63" t="s">
+        <v>62</v>
+      </c>
+      <c r="J63" t="s">
+        <v>60</v>
+      </c>
+      <c r="K63" t="s">
+        <v>78</v>
+      </c>
+      <c r="L63" t="s">
+        <v>99</v>
+      </c>
+      <c r="M63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64" s="1">
+        <f>F56*F58/F65</f>
+        <v>18.666</v>
+      </c>
+      <c r="G64" s="1">
+        <f>G56*G58/G65</f>
+        <v>18.582528</v>
+      </c>
+      <c r="H64">
+        <f>H56*H58/H65</f>
+        <v>20.123136000000002</v>
+      </c>
+      <c r="I64">
+        <f>I56*I58/I65</f>
+        <v>20.122367999999998</v>
+      </c>
+      <c r="J64">
+        <f t="shared" ref="J64" si="10">J56*J58/J65</f>
+        <v>21.568665599999999</v>
+      </c>
+      <c r="K64">
+        <f t="shared" ref="K64" si="11">K56*K58/K65</f>
+        <v>33.662054400000002</v>
+      </c>
+      <c r="L64">
+        <f t="shared" ref="L64:M64" si="12">L56*L58/L65</f>
+        <v>28.603084800000001</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="12"/>
+        <v>20.781465600000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
         <v>7</v>
       </c>
-      <c r="F63">
+      <c r="F65">
         <v>64</v>
       </c>
-      <c r="G63">
+      <c r="G65">
         <v>500</v>
       </c>
-      <c r="H63">
+      <c r="H65">
         <v>500</v>
       </c>
-      <c r="I63">
+      <c r="I65">
         <v>500</v>
       </c>
-      <c r="J63" t="s">
-        <v>59</v>
-      </c>
-      <c r="K63" t="s">
-        <v>59</v>
-      </c>
-      <c r="L63" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I64" t="s">
+      <c r="J65">
+        <v>5000</v>
+      </c>
+      <c r="K65">
+        <v>5000</v>
+      </c>
+      <c r="L65">
+        <v>5000</v>
+      </c>
+      <c r="M65">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F66" s="1"/>
+      <c r="I66" t="s">
         <v>61</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K66" t="s">
         <v>77</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L66" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L65" t="s">
+      <c r="M66" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="M67" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="2" t="s">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E72" t="s">
         <v>9</v>
       </c>
-      <c r="F68">
-        <v>1</v>
-      </c>
-      <c r="G68">
-        <v>1</v>
-      </c>
-      <c r="H68">
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
         <v>2</v>
       </c>
-      <c r="J68">
+      <c r="J72">
         <v>4</v>
       </c>
-      <c r="K68">
+      <c r="K72">
         <v>20</v>
       </c>
-      <c r="L68">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="L72">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E73" t="s">
         <v>10</v>
       </c>
-      <c r="F69">
-        <v>1</v>
-      </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="H69">
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
         <v>2</v>
       </c>
-      <c r="J69">
+      <c r="J73">
         <v>4</v>
       </c>
-      <c r="K69">
+      <c r="K73">
         <v>20</v>
       </c>
-      <c r="L69">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="L73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>55</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E74" t="s">
         <v>11</v>
       </c>
-      <c r="F70">
-        <v>16</v>
-      </c>
-      <c r="G70">
-        <v>16</v>
-      </c>
-      <c r="H70">
-        <v>16</v>
-      </c>
-      <c r="J70">
-        <v>16</v>
-      </c>
-      <c r="K70">
-        <v>16</v>
-      </c>
-      <c r="L70">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="F74">
+        <v>16</v>
+      </c>
+      <c r="G74">
+        <v>16</v>
+      </c>
+      <c r="H74">
+        <v>16</v>
+      </c>
+      <c r="J74">
+        <v>16</v>
+      </c>
+      <c r="K74">
+        <v>16</v>
+      </c>
+      <c r="L74">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>65</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E75" t="s">
         <v>12</v>
       </c>
-      <c r="F71">
-        <f>F70*F69</f>
-        <v>16</v>
-      </c>
-      <c r="G71">
-        <f t="shared" ref="G71" si="9">G70*G69</f>
-        <v>16</v>
-      </c>
-      <c r="H71">
-        <f t="shared" ref="H71" si="10">H70*H69</f>
+      <c r="F75">
+        <f>F74*F73</f>
+        <v>16</v>
+      </c>
+      <c r="G75">
+        <f t="shared" ref="G75" si="13">G74*G73</f>
+        <v>16</v>
+      </c>
+      <c r="H75">
+        <f t="shared" ref="H75" si="14">H74*H73</f>
         <v>32</v>
       </c>
-      <c r="J71">
-        <f>J70*J69</f>
+      <c r="J75">
+        <f>J74*J73</f>
         <v>64</v>
       </c>
-      <c r="K71">
-        <f>K70*K69</f>
+      <c r="K75">
+        <f>K74*K73</f>
         <v>320</v>
       </c>
-      <c r="L71">
-        <f>L70*L69</f>
+      <c r="L75">
+        <f>L74*L73</f>
         <v>256</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="76" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>90</v>
       </c>
-      <c r="B72" s="4">
-        <v>16</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="B76" s="4">
+        <v>16</v>
+      </c>
+      <c r="E76" t="s">
         <v>13</v>
       </c>
-      <c r="F72">
+      <c r="F76">
         <v>1.4516</v>
       </c>
-      <c r="G72">
+      <c r="G76">
         <v>11.061299999999999</v>
       </c>
-      <c r="H72">
+      <c r="H76">
         <v>6.0278999999999998</v>
       </c>
-      <c r="J72">
+      <c r="J76">
         <v>32.767200000000003</v>
       </c>
-      <c r="K72" s="3" t="s">
+      <c r="K76" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L72" s="3">
+      <c r="L76" s="3">
         <v>13.1717</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
         <v>14</v>
       </c>
-      <c r="F73">
-        <f>60*F72</f>
+      <c r="F77">
+        <f>60*F76</f>
         <v>87.096000000000004</v>
       </c>
-      <c r="G73">
-        <f>60*G72</f>
+      <c r="G77">
+        <f>60*G76</f>
         <v>663.678</v>
       </c>
-      <c r="H73">
-        <f t="shared" ref="H73" si="11">60*H72</f>
+      <c r="H77">
+        <f t="shared" ref="H77" si="15">60*H76</f>
         <v>361.67399999999998</v>
       </c>
-      <c r="J73">
-        <f>60*J72</f>
+      <c r="J77">
+        <f>60*J76</f>
         <v>1966.0320000000002</v>
       </c>
-      <c r="K73" s="5">
+      <c r="K77" s="5">
         <f>60*15</f>
         <v>900</v>
       </c>
-      <c r="L73">
-        <f>60*L72</f>
+      <c r="L77">
+        <f>60*L76</f>
         <v>790.30200000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E74" t="s">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>106</v>
+      </c>
+      <c r="F78">
+        <f>F77*F75*F79/100</f>
+        <v>1117.6158720000001</v>
+      </c>
+      <c r="G78">
+        <f t="shared" ref="G78:L78" si="16">G77*G75*G79/100</f>
+        <v>10167.54696</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="16"/>
+        <v>10276.1710272</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="16"/>
+        <v>107140.87987200002</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="16"/>
+        <v>159753.60000000001</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="16"/>
+        <v>129139.14024959999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
         <v>17</v>
       </c>
-      <c r="F74">
+      <c r="F79">
         <v>80.2</v>
       </c>
-      <c r="G74">
+      <c r="G79">
         <v>95.75</v>
       </c>
-      <c r="H74" s="3">
+      <c r="H79" s="3">
         <v>88.79</v>
       </c>
-      <c r="J74" s="3">
+      <c r="J79" s="3">
         <v>85.15</v>
       </c>
-      <c r="K74" s="1">
+      <c r="K79" s="1">
         <v>55.47</v>
       </c>
-      <c r="L74" s="1">
+      <c r="L79" s="1">
         <v>63.83</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
         <v>92</v>
       </c>
-      <c r="F75">
-        <f>(100/(F68*F70) + 500*(F68-1)/(F68*F70) + 100*$B$72/(F68*F70) + 100*F73)/(1+5+$B$72+F73)</f>
+      <c r="F80">
+        <f>(100/(F72*F74) + 500*(F72-1)/(F72*F74) + 100*$B$76/(F72*F74) + 100*F77)/(1+5+$B$76+F77)</f>
         <v>80.808187284593387</v>
       </c>
-      <c r="G75">
-        <f t="shared" ref="G75:L75" si="12">(100/(G68*G70) + 500*(G68-1)/(G68*G70) + 100*$B$72/(G68*G70) + 100*G73)/(1+5+$B$72+G73)</f>
+      <c r="G80">
+        <f t="shared" ref="G80:L80" si="17">(100/(G72*G74) + 500*(G72-1)/(G72*G74) + 100*$B$76/(G72*G74) + 100*G77)/(1+5+$B$76+G77)</f>
         <v>96.946452999804578</v>
       </c>
-      <c r="H75">
-        <f t="shared" si="12"/>
+      <c r="H80">
+        <f t="shared" si="17"/>
         <v>94.445153958829621</v>
       </c>
-      <c r="J75">
-        <f t="shared" si="12"/>
+      <c r="J80">
+        <f t="shared" si="17"/>
         <v>98.918528474390754</v>
       </c>
-      <c r="K75">
-        <f t="shared" si="12"/>
+      <c r="K80">
+        <f t="shared" si="17"/>
         <v>97.651843817787423</v>
       </c>
-      <c r="L75">
-        <f t="shared" si="12"/>
+      <c r="L80">
+        <f t="shared" si="17"/>
         <v>97.335889238238977</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E76" t="s">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
         <v>18</v>
       </c>
-      <c r="F76">
+      <c r="F81">
         <v>440.02</v>
       </c>
-      <c r="G76">
+      <c r="G81">
         <v>437.05</v>
       </c>
-      <c r="H76">
+      <c r="H81">
         <v>1080</v>
       </c>
-      <c r="J76">
+      <c r="J81">
         <v>2600</v>
       </c>
-      <c r="K76" t="s">
+      <c r="K81" t="s">
         <v>70</v>
       </c>
-      <c r="L76" t="s">
+      <c r="L81" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
         <v>19</v>
       </c>
-      <c r="F77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H77" s="3" t="s">
+      <c r="F82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J77" s="3" t="s">
+      <c r="J82" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K82" t="s">
         <v>71</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L82" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
         <v>7</v>
       </c>
-      <c r="F78">
+      <c r="F83">
         <v>64</v>
       </c>
-      <c r="G78">
+      <c r="G83">
         <v>500</v>
       </c>
-      <c r="H78">
+      <c r="H83">
         <v>500</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J83" t="s">
         <v>59</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K83" t="s">
         <v>72</v>
       </c>
-      <c r="L78" t="s">
+      <c r="L83" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K79" t="s">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K84" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E80" s="1" t="s">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E85" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E81" s="1" t="s">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E88" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M83" s="1" t="s">
+      <c r="M88" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>1</v>
-      </c>
-      <c r="B84" s="2" t="s">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E89" t="s">
         <v>9</v>
       </c>
-      <c r="F84">
+      <c r="F89">
         <v>8</v>
       </c>
-      <c r="G84">
+      <c r="G89">
         <v>8</v>
       </c>
-      <c r="H84">
+      <c r="H89">
         <v>8</v>
       </c>
-      <c r="M84" t="s">
+      <c r="M89" t="s">
         <v>9</v>
       </c>
-      <c r="N84">
+      <c r="N89">
         <v>4</v>
       </c>
-      <c r="O84">
+      <c r="O89">
         <v>10</v>
       </c>
-      <c r="P84">
+      <c r="P89">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E90" t="s">
         <v>10</v>
       </c>
-      <c r="F85">
+      <c r="F90">
         <v>8</v>
       </c>
-      <c r="G85">
+      <c r="G90">
         <v>8</v>
       </c>
-      <c r="H85">
+      <c r="H90">
         <v>8</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M90" t="s">
         <v>10</v>
       </c>
-      <c r="N85">
+      <c r="N90">
         <v>4</v>
       </c>
-      <c r="O85">
+      <c r="O90">
         <v>10</v>
       </c>
-      <c r="P85">
+      <c r="P90">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>66</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E91" t="s">
         <v>11</v>
       </c>
-      <c r="F86">
-        <v>16</v>
-      </c>
-      <c r="G86">
-        <v>16</v>
-      </c>
-      <c r="H86">
-        <v>16</v>
-      </c>
-      <c r="M86" t="s">
+      <c r="F91">
+        <v>16</v>
+      </c>
+      <c r="G91">
+        <v>16</v>
+      </c>
+      <c r="H91">
+        <v>16</v>
+      </c>
+      <c r="M91" t="s">
         <v>11</v>
       </c>
-      <c r="N86">
+      <c r="N91">
         <v>12</v>
       </c>
-      <c r="O86">
+      <c r="O91">
         <v>12</v>
       </c>
-      <c r="P86">
+      <c r="P91">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="4">
-        <v>16</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="B92" s="4">
+        <v>16</v>
+      </c>
+      <c r="E92" t="s">
         <v>12</v>
       </c>
-      <c r="F87">
-        <f>F86*F85</f>
+      <c r="F92">
+        <f>F91*F90</f>
         <v>128</v>
       </c>
-      <c r="G87">
-        <f>G86*G85</f>
+      <c r="G92">
+        <f>G91*G90</f>
         <v>128</v>
       </c>
-      <c r="H87">
-        <f>H86*H85</f>
+      <c r="H92">
+        <f>H91*H90</f>
         <v>128</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M92" t="s">
         <v>12</v>
       </c>
-      <c r="N87">
-        <f>N86*N85</f>
+      <c r="N92">
+        <f>N91*N90</f>
         <v>48</v>
       </c>
-      <c r="O87">
-        <f>O86*O85</f>
+      <c r="O92">
+        <f>O91*O90</f>
         <v>120</v>
       </c>
-      <c r="P87">
-        <f>P86*P85</f>
+      <c r="P92">
+        <f>P91*P90</f>
         <v>120</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E88" t="s">
-        <v>13</v>
-      </c>
-      <c r="F88">
-        <v>9.6265000000000001</v>
-      </c>
-      <c r="G88" s="1">
-        <v>8.9794</v>
-      </c>
-      <c r="H88">
-        <v>8.7073999999999998</v>
-      </c>
-      <c r="M88" t="s">
-        <v>13</v>
-      </c>
-      <c r="N88">
-        <v>4.8578000000000001</v>
-      </c>
-      <c r="O88" s="3">
-        <v>4.3205999999999998</v>
-      </c>
-      <c r="P88">
-        <v>4.3733000000000004</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E89" t="s">
-        <v>14</v>
-      </c>
-      <c r="F89">
-        <f>60*F88</f>
-        <v>577.59</v>
-      </c>
-      <c r="G89">
-        <f>60*G88</f>
-        <v>538.76400000000001</v>
-      </c>
-      <c r="H89">
-        <f>60*H88</f>
-        <v>522.44399999999996</v>
-      </c>
-      <c r="M89" t="s">
-        <v>14</v>
-      </c>
-      <c r="N89">
-        <f>60*N88</f>
-        <v>291.46800000000002</v>
-      </c>
-      <c r="O89">
-        <f>60*O88</f>
-        <v>259.23599999999999</v>
-      </c>
-      <c r="P89">
-        <f>60*P88</f>
-        <v>262.39800000000002</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E90" t="s">
-        <v>17</v>
-      </c>
-      <c r="F90" s="1">
-        <v>75.48</v>
-      </c>
-      <c r="G90" s="1">
-        <v>73.37</v>
-      </c>
-      <c r="H90">
-        <v>75.66</v>
-      </c>
-      <c r="M90" t="s">
-        <v>17</v>
-      </c>
-      <c r="N90" s="3">
-        <v>83.57</v>
-      </c>
-      <c r="O90" s="1">
-        <v>74.53</v>
-      </c>
-      <c r="P90">
-        <v>75.33</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E91" t="s">
-        <v>92</v>
-      </c>
-      <c r="F91">
-        <f>(100/(F84*F86) + 500*(F84-1)/(F84*F86) + 100*$B$87/(F84*F86) + 100*F89)/(1+5+$B$87+F89)</f>
-        <v>96.398580696809475</v>
-      </c>
-      <c r="G91">
-        <f>(100/(G84*G86) + 500*(G84-1)/(G84*G86) + 100*$B$87/(G84*G86) + 100*G89)/(1+5+$B$87+G89)</f>
-        <v>96.149226769193461</v>
-      </c>
-      <c r="H91">
-        <f>(100/(G84*G86) + 500*(G84-1)/(G84*G86) + 100*$B$87/(G84*G86) + 100*G89)/(1+5+$B$87+G89)</f>
-        <v>96.149226769193461</v>
-      </c>
-      <c r="M91" t="s">
-        <v>91</v>
-      </c>
-      <c r="N91">
-        <f>(100/(N84*N86) + 500*(N84-1)/(N84*N86) + 100*$B$87/(N84*N86) + 100*N89)/(1+5+$B$87+N89)</f>
-        <v>93.194414315549494</v>
-      </c>
-      <c r="O91">
-        <f>(100/(O84*O86) + 500*(O84-1)/(O84*O86) + 100*$B$87/(O84*O86) + 100*O89)/(1+5+$B$87+O89)</f>
-        <v>92.361101234076244</v>
-      </c>
-      <c r="P91">
-        <f>(100/(P84*P86) + 500*(P84-1)/(P84*P86) + 100*$B$87/(P84*P86) + 100*P89)/(1+5+$B$87+P89)</f>
-        <v>92.446032203695765</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E92" t="s">
-        <v>18</v>
-      </c>
-      <c r="F92">
-        <v>5350</v>
-      </c>
-      <c r="G92">
-        <v>5430</v>
-      </c>
-      <c r="H92">
-        <v>5310</v>
-      </c>
-      <c r="M92" t="s">
-        <v>18</v>
-      </c>
-      <c r="N92">
-        <v>2330</v>
-      </c>
-      <c r="O92">
-        <v>8600</v>
-      </c>
-      <c r="P92">
-        <v>8570</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="s">
-        <v>81</v>
-      </c>
-      <c r="G93" t="s">
-        <v>95</v>
-      </c>
-      <c r="H93" t="s">
-        <v>104</v>
+        <v>13</v>
+      </c>
+      <c r="F93">
+        <v>9.6265000000000001</v>
+      </c>
+      <c r="G93" s="1">
+        <v>8.9794</v>
+      </c>
+      <c r="H93">
+        <v>8.7073999999999998</v>
       </c>
       <c r="M93" t="s">
-        <v>19</v>
-      </c>
-      <c r="N93" t="s">
-        <v>85</v>
-      </c>
-      <c r="O93" t="s">
-        <v>88</v>
-      </c>
-      <c r="P93" t="s">
-        <v>94</v>
+        <v>13</v>
+      </c>
+      <c r="N93">
+        <v>4.8578000000000001</v>
+      </c>
+      <c r="O93" s="3">
+        <v>4.3205999999999998</v>
+      </c>
+      <c r="P93">
+        <v>4.3733000000000004</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" t="s">
-        <v>80</v>
-      </c>
-      <c r="G94" t="s">
-        <v>80</v>
-      </c>
-      <c r="H94" t="s">
-        <v>80</v>
+        <v>14</v>
+      </c>
+      <c r="F94">
+        <f>60*F93</f>
+        <v>577.59</v>
+      </c>
+      <c r="G94">
+        <f>60*G93</f>
+        <v>538.76400000000001</v>
+      </c>
+      <c r="H94">
+        <f>60*H93</f>
+        <v>522.44399999999996</v>
       </c>
       <c r="M94" t="s">
-        <v>7</v>
-      </c>
-      <c r="N94" t="s">
-        <v>84</v>
-      </c>
-      <c r="O94" t="s">
-        <v>59</v>
-      </c>
-      <c r="P94" t="s">
-        <v>59</v>
+        <v>14</v>
+      </c>
+      <c r="N94">
+        <f>60*N93</f>
+        <v>291.46800000000002</v>
+      </c>
+      <c r="O94">
+        <f>60*O93</f>
+        <v>259.23599999999999</v>
+      </c>
+      <c r="P94">
+        <f>60*P93</f>
+        <v>262.39800000000002</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
+        <v>106</v>
+      </c>
+      <c r="F95">
+        <f>F94*F92*F96/100</f>
+        <v>55803.511296000004</v>
+      </c>
+      <c r="G95">
+        <f t="shared" ref="G95:H95" si="18">G94*G92*G96/100</f>
+        <v>50597.266790400005</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="18"/>
+        <v>50595.984691199992</v>
+      </c>
+      <c r="M95" t="s">
+        <v>106</v>
+      </c>
+      <c r="N95">
+        <f t="shared" ref="N95" si="19">N94*N92*N96/100</f>
+        <v>11691.830764799997</v>
+      </c>
+      <c r="O95">
+        <f t="shared" ref="O95" si="20">O94*O92*O96/100</f>
+        <v>23185.030896</v>
+      </c>
+      <c r="P95">
+        <f>P94*P92*P96/100</f>
+        <v>23719.729608000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>17</v>
+      </c>
+      <c r="F96" s="1">
+        <v>75.48</v>
+      </c>
+      <c r="G96" s="1">
+        <v>73.37</v>
+      </c>
+      <c r="H96">
+        <v>75.66</v>
+      </c>
+      <c r="M96" t="s">
+        <v>17</v>
+      </c>
+      <c r="N96" s="3">
+        <v>83.57</v>
+      </c>
+      <c r="O96" s="1">
+        <v>74.53</v>
+      </c>
+      <c r="P96">
+        <v>75.33</v>
+      </c>
+    </row>
+    <row r="97" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>92</v>
+      </c>
+      <c r="F97">
+        <f>(100/(F89*F91) + 500*(F89-1)/(F89*F91) + 100*$B$92/(F89*F91) + 100*F94)/(1+5+$B$92+F94)</f>
+        <v>96.398580696809475</v>
+      </c>
+      <c r="G97">
+        <f>(100/(G89*G91) + 500*(G89-1)/(G89*G91) + 100*$B$92/(G89*G91) + 100*G94)/(1+5+$B$92+G94)</f>
+        <v>96.149226769193461</v>
+      </c>
+      <c r="H97">
+        <f>(100/(G89*G91) + 500*(G89-1)/(G89*G91) + 100*$B$92/(G89*G91) + 100*G94)/(1+5+$B$92+G94)</f>
+        <v>96.149226769193461</v>
+      </c>
+      <c r="M97" t="s">
+        <v>91</v>
+      </c>
+      <c r="N97">
+        <f>(100/(N89*N91) + 500*(N89-1)/(N89*N91) + 100*$B$92/(N89*N91) + 100*N94)/(1+5+$B$92+N94)</f>
+        <v>93.194414315549494</v>
+      </c>
+      <c r="O97">
+        <f>(100/(O89*O91) + 500*(O89-1)/(O89*O91) + 100*$B$92/(O89*O91) + 100*O94)/(1+5+$B$92+O94)</f>
+        <v>92.361101234076244</v>
+      </c>
+      <c r="P97">
+        <f>(100/(P89*P91) + 500*(P89-1)/(P89*P91) + 100*$B$92/(P89*P91) + 100*P94)/(1+5+$B$92+P94)</f>
+        <v>92.446032203695765</v>
+      </c>
+    </row>
+    <row r="98" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>18</v>
+      </c>
+      <c r="F98">
+        <v>5350</v>
+      </c>
+      <c r="G98">
+        <v>5430</v>
+      </c>
+      <c r="H98">
+        <v>5310</v>
+      </c>
+      <c r="M98" t="s">
+        <v>18</v>
+      </c>
+      <c r="N98">
+        <v>2330</v>
+      </c>
+      <c r="O98">
+        <v>8600</v>
+      </c>
+      <c r="P98">
+        <v>8570</v>
+      </c>
+    </row>
+    <row r="99" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
+        <v>81</v>
+      </c>
+      <c r="G99" t="s">
+        <v>95</v>
+      </c>
+      <c r="H99" t="s">
+        <v>103</v>
+      </c>
+      <c r="M99" t="s">
+        <v>19</v>
+      </c>
+      <c r="N99" t="s">
+        <v>85</v>
+      </c>
+      <c r="O99" t="s">
+        <v>88</v>
+      </c>
+      <c r="P99" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="100" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" t="s">
+        <v>80</v>
+      </c>
+      <c r="G100" t="s">
+        <v>80</v>
+      </c>
+      <c r="H100" t="s">
+        <v>80</v>
+      </c>
+      <c r="M100" t="s">
+        <v>7</v>
+      </c>
+      <c r="N100" t="s">
+        <v>84</v>
+      </c>
+      <c r="O100" t="s">
+        <v>59</v>
+      </c>
+      <c r="P100" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
         <v>86</v>
       </c>
-      <c r="F95">
+      <c r="F101">
         <v>43.73</v>
       </c>
-      <c r="G95">
+      <c r="G101">
         <v>39.61</v>
       </c>
-      <c r="H95">
+      <c r="H101">
         <v>38.47</v>
       </c>
-      <c r="O95" s="1" t="s">
+      <c r="O101" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="P95" t="s">
+      <c r="P101" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G96" t="s">
+    <row r="102" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
         <v>87</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H102" t="s">
         <v>87</v>
       </c>
-      <c r="I96" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="97" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E97" s="1" t="s">
+    </row>
+    <row r="103" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G97" s="1" t="s">
+      <c r="G103" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H97" t="s">
-        <v>103</v>
+      <c r="H103" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>